<commit_message>
done renaming in transport optimization
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/TransportSampleDataReverse.xlsx
+++ b/pyloghub/sample_data/TransportSampleDataReverse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21342874-4A7B-4008-AEE4-109E3D5D0204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8417B022-01F1-4C37-BF8E-C0752FB9EE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4E1632C1-AC35-4061-AA24-2141855F7E66}"/>
   </bookViews>
@@ -280,36 +280,18 @@
     <t>maxCapacityVolume</t>
   </si>
   <si>
-    <t>maxCapacityLoadingMeter</t>
-  </si>
-  <si>
     <t>fixedCosts</t>
   </si>
   <si>
     <t>costsPerStop</t>
   </si>
   <si>
-    <t>costsPerKm</t>
-  </si>
-  <si>
-    <t>sender</t>
-  </si>
-  <si>
-    <t>senderServiceTime</t>
-  </si>
-  <si>
     <t>earliestPickupTime</t>
   </si>
   <si>
     <t>latestPickupTime</t>
   </si>
   <si>
-    <t>recipient</t>
-  </si>
-  <si>
-    <t>recipientServiceTime</t>
-  </si>
-  <si>
     <t>earliestDeliveryTime</t>
   </si>
   <si>
@@ -322,13 +304,31 @@
     <t>volume</t>
   </si>
   <si>
-    <t>loadingMeter</t>
-  </si>
-  <si>
-    <t>opportunityCosts</t>
-  </si>
-  <si>
     <t>vehicleType</t>
+  </si>
+  <si>
+    <t>maxCapacityPallets</t>
+  </si>
+  <si>
+    <t>costsPerDistanceUnit</t>
+  </si>
+  <si>
+    <t>senderId</t>
+  </si>
+  <si>
+    <t>recipientId</t>
+  </si>
+  <si>
+    <t>recipientStopDuration</t>
+  </si>
+  <si>
+    <t>pallets</t>
+  </si>
+  <si>
+    <t>externalCosts</t>
+  </si>
+  <si>
+    <t>senderStopDuration</t>
   </si>
 </sst>
 </file>
@@ -445,10 +445,10 @@
     <tableColumn id="8" xr3:uid="{100F75B2-417D-47B8-98B4-A4F3C15AF815}" name="maxRouteDuration"/>
     <tableColumn id="9" xr3:uid="{79023D3E-A627-4810-ABD3-407A8DAD11B8}" name="maxCapacityWeight"/>
     <tableColumn id="10" xr3:uid="{3BCB04DD-328E-48B1-A388-58D447784D5C}" name="maxCapacityVolume"/>
-    <tableColumn id="11" xr3:uid="{68F68E86-A30E-4FAB-9BBD-CC7C97D52574}" name="maxCapacityLoadingMeter"/>
+    <tableColumn id="11" xr3:uid="{68F68E86-A30E-4FAB-9BBD-CC7C97D52574}" name="maxCapacityPallets"/>
     <tableColumn id="12" xr3:uid="{3C93EB62-AD01-4957-8BCA-B799A2810B52}" name="fixedCosts"/>
     <tableColumn id="13" xr3:uid="{D9B2FF8D-3CCA-42E2-B4EC-AF2834CD8FB2}" name="costsPerStop"/>
-    <tableColumn id="14" xr3:uid="{3F145C36-DB7C-41BD-ABCD-BB95B9422E2F}" name="costsPerKm"/>
+    <tableColumn id="14" xr3:uid="{3F145C36-DB7C-41BD-ABCD-BB95B9422E2F}" name="costsPerDistanceUnit"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -460,18 +460,18 @@
   <tableColumns count="15">
     <tableColumn id="15" xr3:uid="{F742AB11-9F7B-402D-846A-6DBFFCF9BE8E}" name="id"/>
     <tableColumn id="1" xr3:uid="{06EF1A47-B09F-4657-8D76-C7295050EC83}" name="name"/>
-    <tableColumn id="2" xr3:uid="{B873AB19-105A-4140-A893-C7CE3DB9FD7E}" name="sender"/>
-    <tableColumn id="3" xr3:uid="{CFE63877-5321-4CF0-8709-C77A4A25F5C9}" name="senderServiceTime"/>
+    <tableColumn id="2" xr3:uid="{B873AB19-105A-4140-A893-C7CE3DB9FD7E}" name="senderId"/>
+    <tableColumn id="3" xr3:uid="{CFE63877-5321-4CF0-8709-C77A4A25F5C9}" name="senderStopDuration"/>
     <tableColumn id="4" xr3:uid="{52DE6885-B3B3-40B2-8282-EA9481224001}" name="earliestPickupTime" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{950FFAA0-65E5-47FB-BC56-110D1CF01BBC}" name="latestPickupTime" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{2188F77B-F7E4-4E51-8545-0EB32B553029}" name="recipient"/>
-    <tableColumn id="7" xr3:uid="{7E336A27-1396-4262-90E2-1D1D0A94C1C7}" name="recipientServiceTime"/>
+    <tableColumn id="6" xr3:uid="{2188F77B-F7E4-4E51-8545-0EB32B553029}" name="recipientId"/>
+    <tableColumn id="7" xr3:uid="{7E336A27-1396-4262-90E2-1D1D0A94C1C7}" name="recipientStopDuration"/>
     <tableColumn id="8" xr3:uid="{494E36CC-27FE-4D05-9D55-D0FAA85A0A56}" name="earliestDeliveryTime" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{6B19C2FD-9477-42EB-A04D-FA58DFDBD983}" name="latestDeliveryTime" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{D4DE7EE7-8967-439E-999F-4BA7C9D25FA6}" name="weight"/>
     <tableColumn id="11" xr3:uid="{952B1CB7-E1D1-4BFC-9AD9-5D232A00C57A}" name="volume"/>
-    <tableColumn id="12" xr3:uid="{5A625F59-CDC5-4721-9048-709CDDE1840B}" name="loadingMeter"/>
-    <tableColumn id="13" xr3:uid="{DF9E4291-C93A-47F3-8356-E91A6D3599EA}" name="opportunityCosts"/>
+    <tableColumn id="12" xr3:uid="{5A625F59-CDC5-4721-9048-709CDDE1840B}" name="pallets"/>
+    <tableColumn id="13" xr3:uid="{DF9E4291-C93A-47F3-8356-E91A6D3599EA}" name="externalCosts"/>
     <tableColumn id="14" xr3:uid="{2CC5B429-03AF-49B4-A2B5-FFF581EC8C38}" name="vehicleType"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1560,7 +1560,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O2"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,16 +1600,16 @@
         <v>79</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1672,7 +1672,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,34 +1691,34 @@
         <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>94</v>
@@ -1727,7 +1727,7 @@
         <v>95</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>